<commit_message>
ofc pc : Practice
</commit_message>
<xml_diff>
--- a/State_Machine/Output.xlsx
+++ b/State_Machine/Output.xlsx
@@ -344,7 +344,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -354,13 +354,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
-        <v>45218.436076388891</v>
+        <v>45219.45045138889</v>
       </c>
       <c r="D1">
         <v>1</v>

</xml_diff>

<commit_message>
from ofc pc: practice
</commit_message>
<xml_diff>
--- a/State_Machine/Output.xlsx
+++ b/State_Machine/Output.xlsx
@@ -344,7 +344,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -352,7 +352,7 @@
     <col min="3" max="3" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1">
       <c r="A1">
         <v>5</v>
       </c>
@@ -360,7 +360,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1">
-        <v>45219.45045138889</v>
+        <v>45231.640798611108</v>
       </c>
       <c r="D1">
         <v>1</v>

</xml_diff>